<commit_message>
Adjusting Format in Excel File
</commit_message>
<xml_diff>
--- a/Emad_Hanna_Week6_Homework6_Sorting_Algorithm_Results.xlsx
+++ b/Emad_Hanna_Week6_Homework6_Sorting_Algorithm_Results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Private\Drexel\CS502\Week 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\eclipse-workspace\SortingMethods\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -49,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -121,7 +121,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1952,7 +1952,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F16"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1961,6 +1961,7 @@
     <col min="2" max="2" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6">

</xml_diff>